<commit_message>
some minor fixes and information added
</commit_message>
<xml_diff>
--- a/other/planning.xlsx
+++ b/other/planning.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
   <si>
     <t>Plano</t>
   </si>
@@ -137,16 +137,7 @@
     <t>Real (para além do plano)</t>
   </si>
   <si>
-    <t>Estudo do estado da arte</t>
-  </si>
-  <si>
     <t>Levantamento de requisitos</t>
-  </si>
-  <si>
-    <t>Construção do ambiente cloud</t>
-  </si>
-  <si>
-    <t>Integração de ferramentas</t>
   </si>
   <si>
     <t>Relatório intermédio</t>
@@ -266,13 +257,52 @@
     <t xml:space="preserve">Student leaves for employment / fails to complete on time
 fails to complete on time
 </t>
+  </si>
+  <si>
+    <t>Estado da arte</t>
+  </si>
+  <si>
+    <t>Contacto com tecnologias de Virtualização</t>
+  </si>
+  <si>
+    <t>Aplicações para a Cloud</t>
+  </si>
+  <si>
+    <t>Desafios de Segurança e Confiabilidade</t>
+  </si>
+  <si>
+    <t>Formulação clara e concisa dos objetivos a alcançar</t>
+  </si>
+  <si>
+    <t>Seleção da plataforma de virtualização</t>
+  </si>
+  <si>
+    <t>Instalação da plataforma de virtualização</t>
+  </si>
+  <si>
+    <t>Integração de ferramentas de avaliação</t>
+  </si>
+  <si>
+    <t>Introdução de falhas muito simples</t>
+  </si>
+  <si>
+    <t>Preparar apresentação pública para discussão</t>
+  </si>
+  <si>
+    <t>Descrever trabalho a realizar no semestre seguinte</t>
+  </si>
+  <si>
+    <t>Construção do ambiente Cloud</t>
+  </si>
+  <si>
+    <t>Experiências com as ferramentas e resultados</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -356,6 +386,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -617,7 +654,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -675,62 +712,65 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="7" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="9" fillId="8" borderId="3" xfId="3" applyFill="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="8" borderId="3" xfId="3" applyFill="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -743,27 +783,7 @@
     <cellStyle name="Period Highlight Control" xfId="7"/>
     <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="7"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <fill>
         <patternFill>
@@ -1412,16 +1432,16 @@
   <sheetPr codeName="Folha1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:BQ13"/>
+  <dimension ref="B2:BQ23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="28.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.5" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.25" style="1" customWidth="1"/>
     <col min="4" max="4" width="7.75" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.25" style="1" customWidth="1"/>
@@ -1432,26 +1452,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:69" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
+      <c r="B2" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
     </row>
     <row r="3" spans="2:69" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
       <c r="K3" s="8" t="s">
         <v>12</v>
       </c>
@@ -1494,14 +1514,14 @@
       </c>
     </row>
     <row r="4" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
       <c r="AT4" s="1"/>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
@@ -1559,78 +1579,78 @@
         <v>7</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="29"/>
+      <c r="W7" s="29"/>
+      <c r="X7" s="29"/>
+      <c r="Y7" s="29"/>
+      <c r="Z7" s="29"/>
+      <c r="AA7" s="29"/>
+      <c r="AB7" s="29"/>
+      <c r="AC7" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD7" s="31"/>
+      <c r="AE7" s="31"/>
+      <c r="AF7" s="31"/>
+      <c r="AG7" s="31"/>
+      <c r="AH7" s="31"/>
+      <c r="AI7" s="31"/>
+      <c r="AJ7" s="31"/>
+      <c r="AK7" s="31"/>
+      <c r="AL7" s="31"/>
+      <c r="AM7" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="22" t="s">
+      <c r="AN7" s="29"/>
+      <c r="AO7" s="29"/>
+      <c r="AP7" s="29"/>
+      <c r="AQ7" s="29"/>
+      <c r="AR7" s="29"/>
+      <c r="AS7" s="29"/>
+      <c r="AT7" s="29"/>
+      <c r="AU7" s="29"/>
+      <c r="AV7" s="29"/>
+      <c r="AW7" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="T7" s="22"/>
-      <c r="U7" s="22"/>
-      <c r="V7" s="22"/>
-      <c r="W7" s="22"/>
-      <c r="X7" s="22"/>
-      <c r="Y7" s="22"/>
-      <c r="Z7" s="22"/>
-      <c r="AA7" s="22"/>
-      <c r="AB7" s="22"/>
-      <c r="AC7" s="21" t="s">
+      <c r="AX7" s="31"/>
+      <c r="AY7" s="31"/>
+      <c r="AZ7" s="31"/>
+      <c r="BA7" s="31"/>
+      <c r="BB7" s="31"/>
+      <c r="BC7" s="31"/>
+      <c r="BD7" s="31"/>
+      <c r="BE7" s="31"/>
+      <c r="BF7" s="31"/>
+      <c r="BG7" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="AD7" s="21"/>
-      <c r="AE7" s="21"/>
-      <c r="AF7" s="21"/>
-      <c r="AG7" s="21"/>
-      <c r="AH7" s="21"/>
-      <c r="AI7" s="21"/>
-      <c r="AJ7" s="21"/>
-      <c r="AK7" s="21"/>
-      <c r="AL7" s="21"/>
-      <c r="AM7" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="AN7" s="22"/>
-      <c r="AO7" s="22"/>
-      <c r="AP7" s="22"/>
-      <c r="AQ7" s="22"/>
-      <c r="AR7" s="22"/>
-      <c r="AS7" s="22"/>
-      <c r="AT7" s="22"/>
-      <c r="AU7" s="22"/>
-      <c r="AV7" s="22"/>
-      <c r="AW7" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="AX7" s="21"/>
-      <c r="AY7" s="21"/>
-      <c r="AZ7" s="21"/>
-      <c r="BA7" s="21"/>
-      <c r="BB7" s="21"/>
-      <c r="BC7" s="21"/>
-      <c r="BD7" s="21"/>
-      <c r="BE7" s="21"/>
-      <c r="BF7" s="21"/>
-      <c r="BG7" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="BH7" s="22"/>
-      <c r="BI7" s="22"/>
-      <c r="BJ7" s="22"/>
-      <c r="BK7" s="22"/>
-      <c r="BL7" s="22"/>
-      <c r="BM7" s="22"/>
-      <c r="BN7" s="22"/>
-      <c r="BO7" s="22"/>
-      <c r="BP7" s="22"/>
+      <c r="BH7" s="29"/>
+      <c r="BI7" s="29"/>
+      <c r="BJ7" s="29"/>
+      <c r="BK7" s="29"/>
+      <c r="BL7" s="29"/>
+      <c r="BM7" s="29"/>
+      <c r="BN7" s="29"/>
+      <c r="BO7" s="29"/>
+      <c r="BP7" s="29"/>
     </row>
     <row r="8" spans="2:69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
@@ -1640,34 +1660,34 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="20">
+      <c r="I8" s="19">
         <v>1</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="19">
         <v>2</v>
       </c>
-      <c r="K8" s="20">
+      <c r="K8" s="19">
         <v>3</v>
       </c>
-      <c r="L8" s="20">
+      <c r="L8" s="19">
         <v>4</v>
       </c>
-      <c r="M8" s="20">
+      <c r="M8" s="19">
         <v>5</v>
       </c>
-      <c r="N8" s="20">
+      <c r="N8" s="19">
         <v>6</v>
       </c>
-      <c r="O8" s="20">
+      <c r="O8" s="19">
         <v>7</v>
       </c>
-      <c r="P8" s="20">
+      <c r="P8" s="19">
         <v>8</v>
       </c>
-      <c r="Q8" s="20">
+      <c r="Q8" s="19">
         <v>9</v>
       </c>
-      <c r="R8" s="20">
+      <c r="R8" s="19">
         <v>10</v>
       </c>
       <c r="S8" s="3">
@@ -1700,34 +1720,34 @@
       <c r="AB8" s="3">
         <v>20</v>
       </c>
-      <c r="AC8" s="20">
+      <c r="AC8" s="19">
         <v>21</v>
       </c>
-      <c r="AD8" s="20">
+      <c r="AD8" s="19">
         <v>22</v>
       </c>
-      <c r="AE8" s="20">
+      <c r="AE8" s="19">
         <v>23</v>
       </c>
-      <c r="AF8" s="20">
+      <c r="AF8" s="19">
         <v>24</v>
       </c>
-      <c r="AG8" s="20">
+      <c r="AG8" s="19">
         <v>25</v>
       </c>
-      <c r="AH8" s="20">
+      <c r="AH8" s="19">
         <v>26</v>
       </c>
-      <c r="AI8" s="20">
+      <c r="AI8" s="19">
         <v>27</v>
       </c>
-      <c r="AJ8" s="20">
+      <c r="AJ8" s="19">
         <v>28</v>
       </c>
-      <c r="AK8" s="20">
+      <c r="AK8" s="19">
         <v>29</v>
       </c>
-      <c r="AL8" s="20">
+      <c r="AL8" s="19">
         <v>30</v>
       </c>
       <c r="AM8" s="3">
@@ -1760,34 +1780,34 @@
       <c r="AV8" s="3">
         <v>40</v>
       </c>
-      <c r="AW8" s="20">
+      <c r="AW8" s="19">
         <v>41</v>
       </c>
-      <c r="AX8" s="20">
+      <c r="AX8" s="19">
         <v>42</v>
       </c>
-      <c r="AY8" s="20">
+      <c r="AY8" s="19">
         <v>43</v>
       </c>
-      <c r="AZ8" s="20">
+      <c r="AZ8" s="19">
         <v>44</v>
       </c>
-      <c r="BA8" s="20">
+      <c r="BA8" s="19">
         <v>45</v>
       </c>
-      <c r="BB8" s="20">
+      <c r="BB8" s="19">
         <v>46</v>
       </c>
-      <c r="BC8" s="20">
+      <c r="BC8" s="19">
         <v>47</v>
       </c>
-      <c r="BD8" s="20">
+      <c r="BD8" s="19">
         <v>48</v>
       </c>
-      <c r="BE8" s="20">
+      <c r="BE8" s="19">
         <v>49</v>
       </c>
-      <c r="BF8" s="20">
+      <c r="BF8" s="19">
         <v>50</v>
       </c>
       <c r="BG8" s="3">
@@ -1822,9 +1842,9 @@
       </c>
       <c r="BQ8" s="1"/>
     </row>
-    <row r="9" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="14" t="s">
-        <v>14</v>
+    <row r="9" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="38" t="s">
+        <v>54</v>
       </c>
       <c r="C9" s="15">
         <v>1</v>
@@ -1840,9 +1860,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="14" t="s">
-        <v>15</v>
+    <row r="10" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="38" t="s">
+        <v>14</v>
       </c>
       <c r="C10" s="15">
         <v>1</v>
@@ -1858,53 +1878,153 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="15">
-        <v>11</v>
-      </c>
-      <c r="D11" s="15">
-        <v>30</v>
-      </c>
+    <row r="11" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
-      <c r="G11" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="15">
-        <v>11</v>
-      </c>
-      <c r="D12" s="15">
-        <v>30</v>
-      </c>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
-      <c r="G12" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="15">
-        <v>41</v>
-      </c>
-      <c r="D13" s="15">
-        <v>10</v>
-      </c>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
-      <c r="G13" s="16">
+      <c r="G13" s="16"/>
+    </row>
+    <row r="14" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="16"/>
+    </row>
+    <row r="15" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="15">
+        <v>11</v>
+      </c>
+      <c r="D15" s="15">
+        <v>30</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="16">
         <v>0</v>
       </c>
+    </row>
+    <row r="16" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="16"/>
+    </row>
+    <row r="17" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16"/>
+    </row>
+    <row r="18" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="15">
+        <v>11</v>
+      </c>
+      <c r="D18" s="15">
+        <v>30</v>
+      </c>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="16"/>
+    </row>
+    <row r="20" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="16"/>
+    </row>
+    <row r="21" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="15">
+        <v>41</v>
+      </c>
+      <c r="D21" s="15">
+        <v>10</v>
+      </c>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="16"/>
+    </row>
+    <row r="23" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1916,39 +2036,39 @@
     <mergeCell ref="S7:AB7"/>
     <mergeCell ref="I7:R7"/>
   </mergeCells>
-  <conditionalFormatting sqref="I9:BP13">
-    <cfRule type="expression" dxfId="20" priority="1">
+  <conditionalFormatting sqref="I9:BP23">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>PercentagemConcluída</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="3">
+    <cfRule type="expression" dxfId="18" priority="3">
       <formula>PercentagemConcluídaAlém</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="4">
+    <cfRule type="expression" dxfId="17" priority="4">
       <formula>Real</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="5">
+    <cfRule type="expression" dxfId="16" priority="5">
       <formula>RealAlém</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="6">
+    <cfRule type="expression" dxfId="15" priority="6">
       <formula>Plano</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="7">
+    <cfRule type="expression" dxfId="14" priority="7">
       <formula>I$8=período_selecionado</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="11">
+    <cfRule type="expression" dxfId="13" priority="11">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="12">
+    <cfRule type="expression" dxfId="12" priority="12">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14:BP14">
-    <cfRule type="expression" dxfId="12" priority="2">
+  <conditionalFormatting sqref="B24:BP24">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:BP8">
-    <cfRule type="expression" dxfId="11" priority="8">
+    <cfRule type="expression" dxfId="10" priority="8">
       <formula>I$8=período_selecionado</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2000,7 +2120,7 @@
   <dimension ref="B2:BQ12"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="B9" sqref="B9:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2017,26 +2137,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:69" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
+      <c r="B2" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
     </row>
     <row r="3" spans="2:69" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
       <c r="K3" s="8" t="s">
         <v>12</v>
       </c>
@@ -2079,14 +2199,14 @@
       </c>
     </row>
     <row r="4" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
       <c r="AT4" s="1"/>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
@@ -2144,78 +2264,78 @@
         <v>7</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="29"/>
+      <c r="W7" s="29"/>
+      <c r="X7" s="29"/>
+      <c r="Y7" s="29"/>
+      <c r="Z7" s="29"/>
+      <c r="AA7" s="29"/>
+      <c r="AB7" s="29"/>
+      <c r="AC7" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD7" s="31"/>
+      <c r="AE7" s="31"/>
+      <c r="AF7" s="31"/>
+      <c r="AG7" s="31"/>
+      <c r="AH7" s="31"/>
+      <c r="AI7" s="31"/>
+      <c r="AJ7" s="31"/>
+      <c r="AK7" s="31"/>
+      <c r="AL7" s="31"/>
+      <c r="AM7" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="22" t="s">
+      <c r="AN7" s="29"/>
+      <c r="AO7" s="29"/>
+      <c r="AP7" s="29"/>
+      <c r="AQ7" s="29"/>
+      <c r="AR7" s="29"/>
+      <c r="AS7" s="29"/>
+      <c r="AT7" s="29"/>
+      <c r="AU7" s="29"/>
+      <c r="AV7" s="29"/>
+      <c r="AW7" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="T7" s="22"/>
-      <c r="U7" s="22"/>
-      <c r="V7" s="22"/>
-      <c r="W7" s="22"/>
-      <c r="X7" s="22"/>
-      <c r="Y7" s="22"/>
-      <c r="Z7" s="22"/>
-      <c r="AA7" s="22"/>
-      <c r="AB7" s="22"/>
-      <c r="AC7" s="21" t="s">
+      <c r="AX7" s="31"/>
+      <c r="AY7" s="31"/>
+      <c r="AZ7" s="31"/>
+      <c r="BA7" s="31"/>
+      <c r="BB7" s="31"/>
+      <c r="BC7" s="31"/>
+      <c r="BD7" s="31"/>
+      <c r="BE7" s="31"/>
+      <c r="BF7" s="31"/>
+      <c r="BG7" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="AD7" s="21"/>
-      <c r="AE7" s="21"/>
-      <c r="AF7" s="21"/>
-      <c r="AG7" s="21"/>
-      <c r="AH7" s="21"/>
-      <c r="AI7" s="21"/>
-      <c r="AJ7" s="21"/>
-      <c r="AK7" s="21"/>
-      <c r="AL7" s="21"/>
-      <c r="AM7" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="AN7" s="22"/>
-      <c r="AO7" s="22"/>
-      <c r="AP7" s="22"/>
-      <c r="AQ7" s="22"/>
-      <c r="AR7" s="22"/>
-      <c r="AS7" s="22"/>
-      <c r="AT7" s="22"/>
-      <c r="AU7" s="22"/>
-      <c r="AV7" s="22"/>
-      <c r="AW7" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="AX7" s="21"/>
-      <c r="AY7" s="21"/>
-      <c r="AZ7" s="21"/>
-      <c r="BA7" s="21"/>
-      <c r="BB7" s="21"/>
-      <c r="BC7" s="21"/>
-      <c r="BD7" s="21"/>
-      <c r="BE7" s="21"/>
-      <c r="BF7" s="21"/>
-      <c r="BG7" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="BH7" s="22"/>
-      <c r="BI7" s="22"/>
-      <c r="BJ7" s="22"/>
-      <c r="BK7" s="22"/>
-      <c r="BL7" s="22"/>
-      <c r="BM7" s="22"/>
-      <c r="BN7" s="22"/>
-      <c r="BO7" s="22"/>
-      <c r="BP7" s="22"/>
+      <c r="BH7" s="29"/>
+      <c r="BI7" s="29"/>
+      <c r="BJ7" s="29"/>
+      <c r="BK7" s="29"/>
+      <c r="BL7" s="29"/>
+      <c r="BM7" s="29"/>
+      <c r="BN7" s="29"/>
+      <c r="BO7" s="29"/>
+      <c r="BP7" s="29"/>
     </row>
     <row r="8" spans="2:69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
@@ -2225,34 +2345,34 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="20">
+      <c r="I8" s="19">
         <v>1</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="19">
         <v>2</v>
       </c>
-      <c r="K8" s="20">
+      <c r="K8" s="19">
         <v>3</v>
       </c>
-      <c r="L8" s="20">
+      <c r="L8" s="19">
         <v>4</v>
       </c>
-      <c r="M8" s="20">
+      <c r="M8" s="19">
         <v>5</v>
       </c>
-      <c r="N8" s="20">
+      <c r="N8" s="19">
         <v>6</v>
       </c>
-      <c r="O8" s="20">
+      <c r="O8" s="19">
         <v>7</v>
       </c>
-      <c r="P8" s="20">
+      <c r="P8" s="19">
         <v>8</v>
       </c>
-      <c r="Q8" s="20">
+      <c r="Q8" s="19">
         <v>9</v>
       </c>
-      <c r="R8" s="20">
+      <c r="R8" s="19">
         <v>10</v>
       </c>
       <c r="S8" s="3">
@@ -2285,34 +2405,34 @@
       <c r="AB8" s="3">
         <v>20</v>
       </c>
-      <c r="AC8" s="20">
+      <c r="AC8" s="19">
         <v>21</v>
       </c>
-      <c r="AD8" s="20">
+      <c r="AD8" s="19">
         <v>22</v>
       </c>
-      <c r="AE8" s="20">
+      <c r="AE8" s="19">
         <v>23</v>
       </c>
-      <c r="AF8" s="20">
+      <c r="AF8" s="19">
         <v>24</v>
       </c>
-      <c r="AG8" s="20">
+      <c r="AG8" s="19">
         <v>25</v>
       </c>
-      <c r="AH8" s="20">
+      <c r="AH8" s="19">
         <v>26</v>
       </c>
-      <c r="AI8" s="20">
+      <c r="AI8" s="19">
         <v>27</v>
       </c>
-      <c r="AJ8" s="20">
+      <c r="AJ8" s="19">
         <v>28</v>
       </c>
-      <c r="AK8" s="20">
+      <c r="AK8" s="19">
         <v>29</v>
       </c>
-      <c r="AL8" s="20">
+      <c r="AL8" s="19">
         <v>30</v>
       </c>
       <c r="AM8" s="3">
@@ -2345,34 +2465,34 @@
       <c r="AV8" s="3">
         <v>40</v>
       </c>
-      <c r="AW8" s="20">
+      <c r="AW8" s="19">
         <v>41</v>
       </c>
-      <c r="AX8" s="20">
+      <c r="AX8" s="19">
         <v>42</v>
       </c>
-      <c r="AY8" s="20">
+      <c r="AY8" s="19">
         <v>43</v>
       </c>
-      <c r="AZ8" s="20">
+      <c r="AZ8" s="19">
         <v>44</v>
       </c>
-      <c r="BA8" s="20">
+      <c r="BA8" s="19">
         <v>45</v>
       </c>
-      <c r="BB8" s="20">
+      <c r="BB8" s="19">
         <v>46</v>
       </c>
-      <c r="BC8" s="20">
+      <c r="BC8" s="19">
         <v>47</v>
       </c>
-      <c r="BD8" s="20">
+      <c r="BD8" s="19">
         <v>48</v>
       </c>
-      <c r="BE8" s="20">
+      <c r="BE8" s="19">
         <v>49</v>
       </c>
-      <c r="BF8" s="20">
+      <c r="BF8" s="19">
         <v>50</v>
       </c>
       <c r="BG8" s="3">
@@ -2409,7 +2529,7 @@
     </row>
     <row r="9" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C9" s="15">
         <v>1</v>
@@ -2425,7 +2545,7 @@
     </row>
     <row r="10" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C10" s="15">
         <v>1</v>
@@ -2441,7 +2561,7 @@
     </row>
     <row r="11" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C11" s="15">
         <v>21</v>
@@ -2457,7 +2577,7 @@
     </row>
     <row r="12" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C12" s="15">
         <v>41</v>
@@ -2482,33 +2602,33 @@
     <mergeCell ref="AW7:BF7"/>
   </mergeCells>
   <conditionalFormatting sqref="I9:BP12">
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>PercentagemConcluída</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>PercentagemConcluídaAlém</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="5">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>Real</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>RealAlém</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>Plano</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="8">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>I$8=período_selecionado</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="10">
+    <cfRule type="expression" dxfId="3" priority="10">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="11">
+    <cfRule type="expression" dxfId="2" priority="11">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:BP13">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2557,7 +2677,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2568,147 +2688,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="C2" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="33"/>
+      <c r="B3" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C3" s="35"/>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="34"/>
+      <c r="B4" s="24" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="C4" s="36"/>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="20"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="33"/>
+      <c r="B7" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="35"/>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="34"/>
+      <c r="B8" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="36"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="32"/>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27"/>
-      <c r="B4" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="33"/>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="23"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="28" t="s">
+      <c r="B9" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="31" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="29" t="s">
+      <c r="C9" s="35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="33"/>
+      <c r="B10" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="32"/>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27"/>
-      <c r="B8" s="30" t="s">
+      <c r="C10" s="35"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="33"/>
+      <c r="B11" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="33"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="29" t="s">
+      <c r="C11" s="35"/>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="34"/>
+      <c r="B12" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="32" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="32"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="29" t="s">
+      <c r="C12" s="36"/>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="32"/>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27"/>
-      <c r="B12" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="33"/>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="37"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="37"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="37"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some fixes and improvements
</commit_message>
<xml_diff>
--- a/other/planning.xlsx
+++ b/other/planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="EsteLivro" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="8085" activeTab="2"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28770" windowHeight="8085" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="gantt 1semestre" sheetId="1" r:id="rId1"/>
@@ -525,7 +525,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -569,6 +569,80 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -773,7 +847,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -849,18 +923,18 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -882,16 +956,34 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2798,10 +2890,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2812,257 +2904,263 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="45" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="36" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="B3" s="27" t="s">
+      <c r="A3" s="37"/>
+      <c r="B3" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="32"/>
+      <c r="C3" s="38"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="33"/>
-      <c r="B4" s="34" t="s">
+      <c r="A4" s="39"/>
+      <c r="B4" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="35"/>
+      <c r="C4" s="41"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="36"/>
+      <c r="C5" s="42"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="36" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="B7" s="27" t="s">
+      <c r="A7" s="37"/>
+      <c r="B7" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="32"/>
+      <c r="C7" s="38"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="33"/>
-      <c r="B8" s="34" t="s">
+      <c r="A8" s="39"/>
+      <c r="B8" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="35"/>
+      <c r="C8" s="41"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="36" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="27" t="s">
+      <c r="A10" s="37"/>
+      <c r="B10" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="32"/>
+      <c r="C10" s="38"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="27" t="s">
+      <c r="A11" s="37"/>
+      <c r="B11" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="32"/>
+      <c r="C11" s="38"/>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="33"/>
-      <c r="B12" s="34" t="s">
+      <c r="A12" s="39"/>
+      <c r="B12" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="35"/>
+      <c r="C12" s="41"/>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="25"/>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="26"/>
+      <c r="B14" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="27"/>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="26"/>
+      <c r="B15" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="27"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="26"/>
+      <c r="B16" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="27"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="26"/>
+      <c r="B17" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="27"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="28"/>
+      <c r="B18" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="29"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="36"/>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="39"/>
+      <c r="B20" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="41"/>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="36"/>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="37"/>
+      <c r="B22" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="38"/>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="39"/>
+      <c r="B23" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="41"/>
+    </row>
+    <row r="24" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B37" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C37" s="36" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="B14" s="27" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="37"/>
+      <c r="B38" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="32"/>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
-      <c r="B15" s="27" t="s">
+      <c r="C38" s="38"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="37"/>
+      <c r="B39" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="32"/>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
-      <c r="B16" s="27" t="s">
+      <c r="C39" s="38"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="37"/>
+      <c r="B40" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="32"/>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
-      <c r="B17" s="27" t="s">
+      <c r="C40" s="38"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="37"/>
+      <c r="B41" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="32"/>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="33"/>
-      <c r="B18" s="34" t="s">
+      <c r="C41" s="38"/>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="39"/>
+      <c r="B42" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="35"/>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" s="30"/>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
-      <c r="B20" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" s="32"/>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
-      <c r="B21" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="C21" s="32"/>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
-      <c r="B22" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" s="32"/>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
-      <c r="B23" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="32"/>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="33"/>
-      <c r="B24" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="C24" s="35"/>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="C25" s="30"/>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="33"/>
-      <c r="B26" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="C26" s="35"/>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="30"/>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
-      <c r="B28" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" s="32"/>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="33"/>
-      <c r="B29" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" s="35"/>
-    </row>
-    <row r="30" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" s="26" t="s">
-        <v>86</v>
-      </c>
+      <c r="C42" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="C13:C18"/>
     <mergeCell ref="A13:A18"/>
-    <mergeCell ref="C13:C18"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="C19:C24"/>
-    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="C37:C42"/>
+    <mergeCell ref="A19:A20"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A6:A8"/>

</xml_diff>